<commit_message>
Re-run of KQ3 with updated data
</commit_message>
<xml_diff>
--- a/data/Pritts_EPC_KQ3_Includes_Histopathology_SK_03212017.xlsx
+++ b/data/Pritts_EPC_KQ3_Includes_Histopathology_SK_03212017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28108"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21080" windowHeight="10040" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25000" windowHeight="14080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataDictionary" sheetId="2" r:id="rId1"/>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11252" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11251" uniqueCount="917">
   <si>
     <t>Line</t>
   </si>
@@ -4739,8 +4739,8 @@
   <dimension ref="A1:AM163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U149" sqref="U149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -21644,7 +21644,7 @@
         <v>729</v>
       </c>
       <c r="H149" s="75">
-        <v>29917</v>
+        <v>4771</v>
       </c>
       <c r="I149" s="47" t="s">
         <v>646</v>
@@ -21671,16 +21671,16 @@
         <v>35</v>
       </c>
       <c r="Q149" s="47">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="R149" s="47">
-        <v>29917</v>
+        <v>4771</v>
       </c>
       <c r="S149" s="47">
-        <v>115</v>
-      </c>
-      <c r="T149" s="47" t="s">
-        <v>731</v>
+        <v>6</v>
+      </c>
+      <c r="T149" s="47">
+        <v>6.4771000000000001</v>
       </c>
       <c r="U149" s="47" t="s">
         <v>529</v>

</xml_diff>